<commit_message>
updated for new polymers
</commit_message>
<xml_diff>
--- a/datasets/raw/SMILES_to_BigSMILES_Conversion_wo_block_copolymer_with_HSPs.xlsx
+++ b/datasets/raw/SMILES_to_BigSMILES_Conversion_wo_block_copolymer_with_HSPs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdehgha2\Desktop\PhD code\PLS-data1\PLS-Dataset\datasets\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45099D0C-BB53-4C80-AC4C-74495544A651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C473B9E8-B08D-4284-B2E7-F528E107D82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -967,7 +967,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="296">
   <si>
     <t>Name</t>
   </si>
@@ -1846,6 +1846,15 @@
   </si>
   <si>
     <t>{&lt;c1ccc(s1)c2sc(c(C(=O)OCCCCCCCCCC)c2C(=O)OCCCCCCCCCC)c3ccc(s3)c4cc5c(c6cc(Cl)c(CC(CC)CCCC)s6)c6sc(cc6c(c6cc(Cl)c(CC(CC)CCCC)s6)c5s4)&gt;}</t>
+  </si>
+  <si>
+    <t>PM6</t>
+  </si>
+  <si>
+    <t>P5TCN-r</t>
+  </si>
+  <si>
+    <t>P5TCN</t>
   </si>
 </sst>
 </file>
@@ -1902,7 +1911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1912,6 +1921,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2741,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4858,6 +4870,48 @@
         <v>5.9</v>
       </c>
     </row>
+    <row r="99" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E99">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F99">
+        <v>1.7</v>
+      </c>
+      <c r="G99">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E100">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F100">
+        <v>3.4</v>
+      </c>
+      <c r="G100">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E101">
+        <v>17.7</v>
+      </c>
+      <c r="F101">
+        <v>3.75</v>
+      </c>
+      <c r="G101">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated for new dataset
</commit_message>
<xml_diff>
--- a/datasets/raw/SMILES_to_BigSMILES_Conversion_wo_block_copolymer_with_HSPs.xlsx
+++ b/datasets/raw/SMILES_to_BigSMILES_Conversion_wo_block_copolymer_with_HSPs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdehgha2\Desktop\PhD code\PLS-data1\PLS-Dataset\datasets\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C473B9E8-B08D-4284-B2E7-F528E107D82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BA8831-A1B3-4A07-9C27-87A41435F590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30045" yWindow="2700" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -967,7 +967,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -1855,6 +1855,15 @@
   </si>
   <si>
     <t>P5TCN</t>
+  </si>
+  <si>
+    <t>FC(C=C1C(C2=C3C=C(*)S2)=C(C=C(C(S4)=CC=C4C5=C(C(C6=C(SC(C(CCCCC)CC)=C6C7=O)C(CCCCC)CC)=O)C7=C(C8=CC=C(*)S8)S5)S9)C9=C3C(S%10)=CC(F)=C%10CC(CC)CCCCC)=C(S1)CC(CC)CCCCC</t>
+  </si>
+  <si>
+    <t>*C1=CC(F)=C(C2=C(F)C=C(C3=C(CC(CCCCCCCC)CCCCCCCCCC)C=C(C4=C(C#N)C=C(C5=CC(CC(CCCCCCCC)CCCCCCCCCC)=C(*)S5)S4)S3)S2)S1</t>
+  </si>
+  <si>
+    <t>*C1=CC(F)=C(C2=C(F)C=C(C3=C(CC(CCCCCCCC)CCCCCCCCCC)C=C(C4=C(C#N)C=C(C5=CC(CC(CCCCCCCC)CCCCCCCCCC)=C(C6=CC=C(C7=CC=C(C8=C(CC(CCCCCCCC)CCCCCCCCCC)C=C(C9=C(C#N)C=C(C%10=CC(CC(CCCCCCCC)CCCCCCCCCC)=C(C%11=CC=C(C%12=CC=C(C%13=C(CC(CCCCCCCC)CCCCCCCCCC)C=C(C%14=C(C#N)C=C(C%15=CC(CC(CCCCCCCC)CCCCCCCCCC)=C(C%16=CC=C(C%17=CC=C(C%18=C(CC(CCCCCCCC)CCCCCCCCCC)C=C(C%19=C(C#N)C=C(C%20=CC(CC(CCCCCCCC)CCCCCCCCCC)=C(*)S%20)S%19)S%18)S%17)S%16)S%15)S%14)S%13)S%12)S%11)S%10)S9)S8)S7)S6)S5)S4)S3)S2)S1</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1924,6 +1933,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2755,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4874,6 +4886,9 @@
       <c r="A99" s="1" t="s">
         <v>293</v>
       </c>
+      <c r="C99" s="5" t="s">
+        <v>296</v>
+      </c>
       <c r="E99">
         <v>17.100000000000001</v>
       </c>
@@ -4888,6 +4903,9 @@
       <c r="A100" s="4" t="s">
         <v>294</v>
       </c>
+      <c r="C100" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="E100">
         <v>16.899999999999999</v>
       </c>
@@ -4901,6 +4919,9 @@
     <row r="101" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>295</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="E101">
         <v>17.7</v>

</xml_diff>